<commit_message>
Modificaciones varias + Correcciones del Word de Entrega
</commit_message>
<xml_diff>
--- a/tests_cases/TPO - PE-10.xlsx
+++ b/tests_cases/TPO - PE-10.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Aplicaciones\Proyectos\TestingAplicaciones-MatrixTesters-TPO\tests_cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7CD5993-2524-4A31-AFC8-A98379661499}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{035A28DA-876C-4A09-BADF-DFD88BC353E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14715" yWindow="5955" windowWidth="24270" windowHeight="11385" activeTab="1" xr2:uid="{DCE1F527-8622-40D5-806A-6A7E2BCE07A3}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="24270" windowHeight="11385" activeTab="1" xr2:uid="{DCE1F527-8622-40D5-806A-6A7E2BCE07A3}"/>
   </bookViews>
   <sheets>
     <sheet name="MT-14" sheetId="1" r:id="rId1"/>
@@ -108,9 +108,6 @@
     <t>MT-14</t>
   </si>
   <si>
-    <t>None</t>
-  </si>
-  <si>
     <t>Clickear Logo</t>
   </si>
   <si>
@@ -162,9 +159,6 @@
     <t>Redirecciona al Banner</t>
   </si>
   <si>
-    <t>Redirecciona al producto "Zapatillas Verdes"</t>
-  </si>
-  <si>
     <t>Desde varias ventanas hacer un clic en el logo</t>
   </si>
   <si>
@@ -174,7 +168,13 @@
     <t>Clic en el producto "T-Shirt 1"</t>
   </si>
   <si>
-    <t>1.1</t>
+    <t>Denise Posklinski</t>
+  </si>
+  <si>
+    <t>Redirecciona al producto "T-Shirt 1</t>
+  </si>
+  <si>
+    <t>1.2</t>
   </si>
 </sst>
 </file>
@@ -463,15 +463,54 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -487,47 +526,8 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -848,7 +848,7 @@
   <dimension ref="A1:W20"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19:F19"/>
+      <selection activeCell="D16" sqref="D16:F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -880,11 +880,11 @@
       <c r="C1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
+      <c r="D1" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
     </row>
     <row r="2" spans="1:23" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
@@ -896,25 +896,25 @@
       <c r="C2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="41" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
+      <c r="D2" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
     </row>
     <row r="3" spans="1:23" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="20"/>
-      <c r="C3" s="21"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="35"/>
       <c r="D3" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="39" t="s">
+      <c r="E3" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="39"/>
+      <c r="F3" s="41"/>
       <c r="G3" s="3"/>
       <c r="I3" s="3"/>
       <c r="K3" s="3"/>
@@ -979,12 +979,12 @@
       <c r="D7" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="25" t="s">
+      <c r="E7" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="25"/>
-    </row>
-    <row r="8" spans="1:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F7" s="38"/>
+    </row>
+    <row r="8" spans="1:23" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="19">
         <v>1</v>
       </c>
@@ -993,20 +993,20 @@
       </c>
       <c r="C8" s="10"/>
       <c r="D8" s="16"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="24"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="37"/>
     </row>
     <row r="9" spans="1:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="16">
         <v>2</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C9" s="10"/>
       <c r="D9" s="16"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="24"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="37"/>
     </row>
     <row r="10" spans="1:23" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10"/>
@@ -1016,110 +1016,117 @@
       <c r="E10" s="10"/>
     </row>
     <row r="11" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="26" t="s">
+      <c r="A11" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="29" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="29"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="29"/>
-      <c r="F11" s="29"/>
+      <c r="B11" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="23"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
     </row>
     <row r="12" spans="1:23" ht="11.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="27"/>
-      <c r="B12" s="29"/>
-      <c r="C12" s="29"/>
-      <c r="D12" s="29"/>
-      <c r="E12" s="29"/>
-      <c r="F12" s="29"/>
+      <c r="A12" s="40"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
     </row>
     <row r="13" spans="1:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="22" t="s">
+      <c r="B13" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="22"/>
+      <c r="C13" s="31"/>
       <c r="D13" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="E13" s="22" t="s">
+      <c r="E13" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="F13" s="22"/>
+      <c r="F13" s="31"/>
     </row>
     <row r="14" spans="1:23" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="1:23" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="37" t="s">
+      <c r="B15" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="38"/>
-      <c r="D15" s="33" t="s">
+      <c r="C15" s="33"/>
+      <c r="D15" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="E15" s="34"/>
-      <c r="F15" s="35"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="29"/>
     </row>
     <row r="16" spans="1:23" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>1</v>
       </c>
-      <c r="B16" s="36" t="s">
+      <c r="B16" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="30"/>
+      <c r="D16" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="36"/>
-      <c r="D16" s="30" t="s">
-        <v>28</v>
-      </c>
-      <c r="E16" s="31"/>
-      <c r="F16" s="32"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="26"/>
     </row>
     <row r="17" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>2</v>
       </c>
-      <c r="B17" s="36" t="s">
+      <c r="B17" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="30"/>
+      <c r="D17" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="36"/>
-      <c r="D17" s="36" t="s">
-        <v>30</v>
-      </c>
-      <c r="E17" s="36"/>
-      <c r="F17" s="36"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30"/>
     </row>
     <row r="18" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
-      <c r="B18" s="28"/>
-      <c r="C18" s="28"/>
-      <c r="D18" s="28"/>
-      <c r="E18" s="28"/>
-      <c r="F18" s="28"/>
+      <c r="B18" s="22"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="22"/>
     </row>
     <row r="19" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
-      <c r="B19" s="28"/>
-      <c r="C19" s="28"/>
-      <c r="D19" s="28"/>
-      <c r="E19" s="28"/>
-      <c r="F19" s="28"/>
+      <c r="B19" s="22"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="22"/>
     </row>
     <row r="20" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
-      <c r="B20" s="28"/>
-      <c r="C20" s="28"/>
-      <c r="D20" s="28"/>
-      <c r="E20" s="28"/>
-      <c r="F20" s="28"/>
+      <c r="B20" s="22"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E8:F8"/>
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="D2:F2"/>
     <mergeCell ref="B20:C20"/>
@@ -1136,13 +1143,6 @@
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="D20:F20"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E8:F8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -1154,7 +1154,7 @@
   <dimension ref="A1:W27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="E3" sqref="E3:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1181,16 +1181,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
+      <c r="D1" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
     </row>
     <row r="2" spans="1:23" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
@@ -1202,25 +1202,25 @@
       <c r="C2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="41" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
+      <c r="D2" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
     </row>
     <row r="3" spans="1:23" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="20"/>
-      <c r="C3" s="21"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="35"/>
       <c r="D3" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="39" t="s">
+      <c r="E3" s="41" t="s">
         <v>45</v>
       </c>
-      <c r="F3" s="39"/>
+      <c r="F3" s="41"/>
       <c r="G3" s="3"/>
       <c r="I3" s="3"/>
       <c r="K3" s="3"/>
@@ -1285,12 +1285,12 @@
       <c r="D7" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="25" t="s">
+      <c r="E7" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="25"/>
-    </row>
-    <row r="8" spans="1:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F7" s="38"/>
+    </row>
+    <row r="8" spans="1:23" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="19">
         <v>1</v>
       </c>
@@ -1299,20 +1299,20 @@
       </c>
       <c r="C8" s="10"/>
       <c r="D8" s="16"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="24"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="37"/>
     </row>
     <row r="9" spans="1:23" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="16">
         <v>2</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C9" s="10"/>
       <c r="D9" s="16"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="24"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="37"/>
     </row>
     <row r="10" spans="1:23" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10"/>
@@ -1322,263 +1322,263 @@
       <c r="E10" s="10"/>
     </row>
     <row r="11" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="26" t="s">
+      <c r="A11" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="29" t="s">
-        <v>42</v>
-      </c>
-      <c r="C11" s="29"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="29"/>
-      <c r="F11" s="29"/>
+      <c r="B11" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="23"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
     </row>
     <row r="12" spans="1:23" ht="11.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="27"/>
-      <c r="B12" s="29"/>
-      <c r="C12" s="29"/>
-      <c r="D12" s="29"/>
-      <c r="E12" s="29"/>
-      <c r="F12" s="29"/>
+      <c r="A12" s="40"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
     </row>
     <row r="13" spans="1:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="22" t="s">
+      <c r="B13" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="22"/>
+      <c r="C13" s="31"/>
       <c r="D13" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="E13" s="22" t="s">
+      <c r="E13" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="F13" s="22"/>
+      <c r="F13" s="31"/>
     </row>
     <row r="14" spans="1:23" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="1:23" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="37" t="s">
+      <c r="B15" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="38"/>
-      <c r="D15" s="33" t="s">
+      <c r="C15" s="33"/>
+      <c r="D15" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="E15" s="34"/>
-      <c r="F15" s="35"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="29"/>
     </row>
     <row r="16" spans="1:23" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>1</v>
       </c>
-      <c r="B16" s="36" t="s">
+      <c r="B16" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="30"/>
+      <c r="D16" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="36"/>
-      <c r="D16" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="E16" s="31"/>
-      <c r="F16" s="32"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="26"/>
     </row>
     <row r="17" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>2</v>
       </c>
-      <c r="B17" s="36" t="s">
-        <v>27</v>
-      </c>
-      <c r="C17" s="36"/>
-      <c r="D17" s="36" t="s">
-        <v>35</v>
-      </c>
-      <c r="E17" s="36"/>
-      <c r="F17" s="36"/>
+      <c r="B17" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="30"/>
+      <c r="D17" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30"/>
     </row>
     <row r="18" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>3</v>
       </c>
-      <c r="B18" s="36" t="s">
+      <c r="B18" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="30"/>
+      <c r="D18" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="36"/>
-      <c r="D18" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="E18" s="31"/>
-      <c r="F18" s="32"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="26"/>
     </row>
     <row r="19" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>4</v>
       </c>
-      <c r="B19" s="36" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" s="36"/>
-      <c r="D19" s="36" t="s">
-        <v>35</v>
-      </c>
-      <c r="E19" s="36"/>
-      <c r="F19" s="36"/>
+      <c r="B19" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="30"/>
+      <c r="D19" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="E19" s="30"/>
+      <c r="F19" s="30"/>
     </row>
     <row r="20" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>5</v>
       </c>
-      <c r="B20" s="36" t="s">
-        <v>38</v>
-      </c>
-      <c r="C20" s="36"/>
-      <c r="D20" s="30" t="s">
+      <c r="B20" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="E20" s="31"/>
-      <c r="F20" s="32"/>
+      <c r="C20" s="30"/>
+      <c r="D20" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="E20" s="25"/>
+      <c r="F20" s="26"/>
     </row>
     <row r="21" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>6</v>
       </c>
-      <c r="B21" s="36" t="s">
-        <v>27</v>
-      </c>
-      <c r="C21" s="36"/>
-      <c r="D21" s="36" t="s">
-        <v>35</v>
-      </c>
-      <c r="E21" s="36"/>
-      <c r="F21" s="36"/>
+      <c r="B21" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" s="30"/>
+      <c r="D21" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="E21" s="30"/>
+      <c r="F21" s="30"/>
     </row>
     <row r="22" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>7</v>
       </c>
-      <c r="B22" s="36" t="s">
-        <v>39</v>
-      </c>
-      <c r="C22" s="36"/>
-      <c r="D22" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="E22" s="31"/>
-      <c r="F22" s="32"/>
+      <c r="B22" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" s="30"/>
+      <c r="D22" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="E22" s="25"/>
+      <c r="F22" s="26"/>
     </row>
     <row r="23" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>8</v>
       </c>
-      <c r="B23" s="36" t="s">
-        <v>27</v>
-      </c>
-      <c r="C23" s="36"/>
-      <c r="D23" s="36" t="s">
-        <v>35</v>
-      </c>
-      <c r="E23" s="36"/>
-      <c r="F23" s="36"/>
+      <c r="B23" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" s="30"/>
+      <c r="D23" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="E23" s="30"/>
+      <c r="F23" s="30"/>
     </row>
     <row r="24" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>9</v>
       </c>
-      <c r="B24" s="36" t="s">
-        <v>43</v>
-      </c>
-      <c r="C24" s="36"/>
-      <c r="D24" s="30" t="s">
-        <v>40</v>
-      </c>
-      <c r="E24" s="31"/>
-      <c r="F24" s="32"/>
+      <c r="B24" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="C24" s="30"/>
+      <c r="D24" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="E24" s="25"/>
+      <c r="F24" s="26"/>
     </row>
     <row r="25" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>10</v>
       </c>
-      <c r="B25" s="36" t="s">
-        <v>27</v>
-      </c>
-      <c r="C25" s="36"/>
-      <c r="D25" s="36" t="s">
-        <v>35</v>
-      </c>
-      <c r="E25" s="36"/>
-      <c r="F25" s="36"/>
+      <c r="B25" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" s="30"/>
+      <c r="D25" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="E25" s="30"/>
+      <c r="F25" s="30"/>
     </row>
     <row r="26" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>11</v>
       </c>
-      <c r="B26" s="36" t="s">
+      <c r="B26" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="C26" s="30"/>
+      <c r="D26" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="C26" s="36"/>
-      <c r="D26" s="30" t="s">
-        <v>41</v>
-      </c>
-      <c r="E26" s="31"/>
-      <c r="F26" s="32"/>
+      <c r="E26" s="25"/>
+      <c r="F26" s="26"/>
     </row>
     <row r="27" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>12</v>
       </c>
-      <c r="B27" s="36" t="s">
-        <v>27</v>
-      </c>
-      <c r="C27" s="36"/>
-      <c r="D27" s="36" t="s">
-        <v>35</v>
-      </c>
-      <c r="E27" s="36"/>
-      <c r="F27" s="36"/>
+      <c r="B27" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27" s="30"/>
+      <c r="D27" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="E27" s="30"/>
+      <c r="F27" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D15:F15"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="D26:F26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="D27:F27"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:F19"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="B11:F12"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="D16:F16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="D20:F20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D22:F22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="D24:F24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="D25:F25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="D26:F26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="D27:F27"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E7:F7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -1586,6 +1586,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101006CB1A51B3A996C44B977E632F6DEC33D" ma:contentTypeVersion="2" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="2bd25917a97534041ca7931abd8cbbac">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="66b336d3-04c8-489c-ac96-6a14a2b4331d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="173f2ba09421de1668a77200cfb94d82" ns2:_="">
     <xsd:import namespace="66b336d3-04c8-489c-ac96-6a14a2b4331d"/>
@@ -1717,22 +1732,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B439C089-9FB7-457D-8B04-4B618FE47EDC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{08D01FAC-C26F-4BC2-8C04-9A91622ABBCA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C5A42DB-190E-47E2-A19E-CF7C61BA992E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1748,21 +1765,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{08D01FAC-C26F-4BC2-8C04-9A91622ABBCA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B439C089-9FB7-457D-8B04-4B618FE47EDC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>